<commit_message>
Day-5 - JavaScript basics: Scope var,let, const keywords covered
</commit_message>
<xml_diff>
--- a/react-project/JavaScript/Topics.xlsx
+++ b/react-project/JavaScript/Topics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6afe25b8f4bd1/Desktop/React/react-development/react-project/JavaScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7B2A3CC-FB58-479F-9266-56BE3809378F}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20065835-589B-4685-BF8A-6003F7E6F4F8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Time Stamps:</t>
   </si>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +587,9 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Day-6 - JavaScript basics: Arrays completed
</commit_message>
<xml_diff>
--- a/react-project/JavaScript/Topics.xlsx
+++ b/react-project/JavaScript/Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6afe25b8f4bd1/Desktop/React/react-development/react-project/JavaScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20065835-589B-4685-BF8A-6003F7E6F4F8}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E47A45D-A50F-4CE8-9394-7DDE8E345969}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Time Stamps:</t>
   </si>
@@ -591,62 +591,65 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Day-7: JavaScript Basics: Objects
</commit_message>
<xml_diff>
--- a/react-project/JavaScript/Topics.xlsx
+++ b/react-project/JavaScript/Topics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6afe25b8f4bd1/Desktop/React/react-development/react-project/JavaScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E47A45D-A50F-4CE8-9394-7DDE8E345969}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEF0AA68-DB94-436B-814C-21B7E054817F}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Time Stamps:</t>
   </si>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,10 +603,16 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Day-8: JavaScript Basics: Classses,JSON,Error Handling
</commit_message>
<xml_diff>
--- a/react-project/JavaScript/Topics.xlsx
+++ b/react-project/JavaScript/Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6afe25b8f4bd1/Desktop/React/react-development/react-project/JavaScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEF0AA68-DB94-436B-814C-21B7E054817F}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B86D5453-B69D-4397-9BDC-2043B71F427A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Time Stamps:</t>
   </si>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,10 +619,16 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Day-9: JavaScript Basics: DOM, without css and html, creating elements and styling them with js only
</commit_message>
<xml_diff>
--- a/react-project/JavaScript/Topics.xlsx
+++ b/react-project/JavaScript/Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6afe25b8f4bd1/Desktop/React/react-development/react-project/JavaScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B86D5453-B69D-4397-9BDC-2043B71F427A}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5A42B63-FC24-4BB0-A2D2-595EB8227567}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Time Stamps:</t>
   </si>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,10 +635,16 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
API - Chapter started
</commit_message>
<xml_diff>
--- a/react-project/JavaScript/Topics.xlsx
+++ b/react-project/JavaScript/Topics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6afe25b8f4bd1/Desktop/React/react-development/react-project/JavaScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6B16FF9-6142-432A-9BE2-602549753FA0}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4549A9A-8C3F-488D-9401-6F244E17A80A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Time Stamps:</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>DONE</t>
-  </si>
-  <si>
-    <t>revise it from objects tomorrow</t>
   </si>
 </sst>
 </file>
@@ -140,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +147,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -166,10 +169,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,9 +662,7 @@
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
Revison and few modification
</commit_message>
<xml_diff>
--- a/react-project/JavaScript/Topics.xlsx
+++ b/react-project/JavaScript/Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6afe25b8f4bd1/Desktop/React/react-development/react-project/JavaScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4549A9A-8C3F-488D-9401-6F244E17A80A}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_F25DC773A252ABDACC1048E6A15F70FE5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12472645-82C8-452B-91AB-EC541BA38B25}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,6 +189,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>